<commit_message>
Adding Notes for the Teraform Associate exam
</commit_message>
<xml_diff>
--- a/Sem06/Exchange/Courses.xlsx
+++ b/Sem06/Exchange/Courses.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25225"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25330"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\PC1\School\ViaUniversityCollege\Sem06\Exchange\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9274B59E-49EE-40F8-873D-1D9F94A4DC0B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{208305AB-830E-4A82-8071-4C9F72FCAC1E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="74">
   <si>
     <t>Courses</t>
   </si>
@@ -205,13 +205,55 @@
   </si>
   <si>
     <t>University of Malta</t>
+  </si>
+  <si>
+    <t>Hanyang University</t>
+  </si>
+  <si>
+    <t>Korea</t>
+  </si>
+  <si>
+    <t>Seoul</t>
+  </si>
+  <si>
+    <t>Machine Learning with Data Mining</t>
+  </si>
+  <si>
+    <t>Data mining is one of the modern statistical processes which results in the discovery of new patterns in data sets. This course pertains to how to understand the concepts of several data mining techniques and to perform data mining analysis. The topics of the course will include decision trees, based upon regression analysis, cluster analysis, discriminant analysis, factor analysis, neural networks, logistic/poisson regression, and support vector machines. Modern statistical software such as R and/or Python along with other languages, as needed, will be used to demonstrate the techniques.</t>
+  </si>
+  <si>
+    <t>300units</t>
+  </si>
+  <si>
+    <t>INE5008</t>
+  </si>
+  <si>
+    <t>Comprehensive Planning 1(URIP)</t>
+  </si>
+  <si>
+    <t>400units</t>
+  </si>
+  <si>
+    <t>Individual and team experience in solving problems that require creative application of knowledge and of planning processes to all aspects of human settlement; emphasis on professional skills including graphics, computer analysis, writing, and presentation; as well as reviews of planning cases.</t>
+  </si>
+  <si>
+    <t>URE4033</t>
+  </si>
+  <si>
+    <t>INTRODUCTION TO ARTIFICIAL INTELLIGENCE</t>
+  </si>
+  <si>
+    <t>APA4055</t>
+  </si>
+  <si>
+    <t>This course covers theories of Artificial Intelligence algorithms essential to the 4th industrial revolution. First, the course covers Machine Learning, Review of linear algebra and random variables, Supervised learning, Unsupervised learning, Cost function, Optimization &amp; Regularization, Linear and Nonlinear regression, Neural model, Deep learning(Basics, algorithms, Practices). Finally, Learn about application examples for artificial intelligence technology.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -225,16 +267,50 @@
       <name val="Source Sans Pro"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="7"/>
+      <color rgb="FF656565"/>
+      <name val="Dotum"/>
+      <family val="2"/>
+      <charset val="129"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="7"/>
+      <color rgb="FF000000"/>
+      <name val="Dotum"/>
+      <family val="2"/>
+      <charset val="129"/>
+    </font>
+    <font>
+      <sz val="7"/>
+      <color rgb="FF000000"/>
+      <name val="Dotum"/>
+      <family val="2"/>
+      <charset val="129"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF0EBEF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="14">
+  <borders count="16">
     <border>
       <left/>
       <right/>
@@ -391,11 +467,39 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFE1E1E1"/>
+      </left>
+      <right style="medium">
+        <color rgb="FFE1E1E1"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFE1E1E1"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FFE1E1E1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFE1E1E1"/>
+      </left>
+      <right style="medium">
+        <color rgb="FFE1E1E1"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFE1E1E1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
@@ -413,6 +517,18 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -693,24 +809,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B1:I32"/>
+  <dimension ref="B1:I59"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E28" sqref="E28"/>
+    <sheetView tabSelected="1" topLeftCell="G33" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="G58" sqref="G58"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="11.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="53.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="34.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="49.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="255.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="53.44140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="34.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="49.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="255.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="2" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="2" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B2" s="1"/>
       <c r="C2" s="2"/>
       <c r="D2" s="2"/>
@@ -720,7 +836,7 @@
       <c r="H2" s="2"/>
       <c r="I2" s="3"/>
     </row>
-    <row r="3" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B3" s="14"/>
       <c r="C3" s="10" t="s">
         <v>54</v>
@@ -734,7 +850,7 @@
       <c r="H3" s="15"/>
       <c r="I3" s="16"/>
     </row>
-    <row r="4" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B4" s="14"/>
       <c r="C4" s="10" t="s">
         <v>12</v>
@@ -748,7 +864,7 @@
       <c r="H4" s="15"/>
       <c r="I4" s="16"/>
     </row>
-    <row r="5" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B5" s="14"/>
       <c r="C5" s="10" t="s">
         <v>53</v>
@@ -762,7 +878,7 @@
       <c r="H5" s="15"/>
       <c r="I5" s="16"/>
     </row>
-    <row r="6" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B6" s="14"/>
       <c r="C6" s="15"/>
       <c r="D6" s="15"/>
@@ -772,7 +888,7 @@
       <c r="H6" s="15"/>
       <c r="I6" s="16"/>
     </row>
-    <row r="7" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B7" s="14"/>
       <c r="C7" s="7" t="s">
         <v>0</v>
@@ -784,7 +900,7 @@
       <c r="H7" s="15"/>
       <c r="I7" s="16"/>
     </row>
-    <row r="8" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B8" s="14"/>
       <c r="C8" s="8" t="s">
         <v>1</v>
@@ -804,7 +920,7 @@
       <c r="H8" s="15"/>
       <c r="I8" s="16"/>
     </row>
-    <row r="9" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B9" s="14"/>
       <c r="C9" s="12" t="s">
         <v>5</v>
@@ -822,7 +938,7 @@
       <c r="H9" s="15"/>
       <c r="I9" s="16"/>
     </row>
-    <row r="10" spans="2:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B10" s="14"/>
       <c r="C10" s="10" t="s">
         <v>6</v>
@@ -842,7 +958,7 @@
       <c r="H10" s="15"/>
       <c r="I10" s="16"/>
     </row>
-    <row r="11" spans="2:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B11" s="14"/>
       <c r="C11" s="10" t="s">
         <v>7</v>
@@ -862,7 +978,7 @@
       <c r="H11" s="15"/>
       <c r="I11" s="16"/>
     </row>
-    <row r="12" spans="2:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B12" s="14"/>
       <c r="C12" s="10" t="s">
         <v>8</v>
@@ -882,7 +998,7 @@
       <c r="H12" s="15"/>
       <c r="I12" s="16"/>
     </row>
-    <row r="13" spans="2:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B13" s="14"/>
       <c r="C13" s="10" t="s">
         <v>9</v>
@@ -902,7 +1018,7 @@
       <c r="H13" s="15"/>
       <c r="I13" s="16"/>
     </row>
-    <row r="14" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B14" s="14"/>
       <c r="C14" s="13" t="s">
         <v>40</v>
@@ -916,7 +1032,7 @@
       <c r="H14" s="15"/>
       <c r="I14" s="16"/>
     </row>
-    <row r="15" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B15" s="4"/>
       <c r="C15" s="5"/>
       <c r="D15" s="5"/>
@@ -926,8 +1042,8 @@
       <c r="H15" s="5"/>
       <c r="I15" s="6"/>
     </row>
-    <row r="17" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="18" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="18" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B18" s="1"/>
       <c r="C18" s="2"/>
       <c r="D18" s="2"/>
@@ -937,7 +1053,7 @@
       <c r="H18" s="2"/>
       <c r="I18" s="3"/>
     </row>
-    <row r="19" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B19" s="14"/>
       <c r="C19" s="10" t="s">
         <v>54</v>
@@ -951,7 +1067,7 @@
       <c r="H19" s="15"/>
       <c r="I19" s="16"/>
     </row>
-    <row r="20" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B20" s="14"/>
       <c r="C20" s="10" t="s">
         <v>12</v>
@@ -965,7 +1081,7 @@
       <c r="H20" s="15"/>
       <c r="I20" s="16"/>
     </row>
-    <row r="21" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B21" s="14"/>
       <c r="C21" s="10" t="s">
         <v>53</v>
@@ -979,7 +1095,7 @@
       <c r="H21" s="15"/>
       <c r="I21" s="16"/>
     </row>
-    <row r="22" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B22" s="14"/>
       <c r="C22" s="15"/>
       <c r="D22" s="15"/>
@@ -989,7 +1105,7 @@
       <c r="H22" s="15"/>
       <c r="I22" s="16"/>
     </row>
-    <row r="23" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B23" s="14"/>
       <c r="C23" s="7" t="s">
         <v>0</v>
@@ -1001,7 +1117,7 @@
       <c r="H23" s="15"/>
       <c r="I23" s="16"/>
     </row>
-    <row r="24" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B24" s="14"/>
       <c r="C24" s="7" t="s">
         <v>1</v>
@@ -1021,7 +1137,7 @@
       <c r="H24" s="15"/>
       <c r="I24" s="16"/>
     </row>
-    <row r="25" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B25" s="14"/>
       <c r="C25" s="12" t="s">
         <v>5</v>
@@ -1039,7 +1155,7 @@
       <c r="H25" s="15"/>
       <c r="I25" s="16"/>
     </row>
-    <row r="26" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B26" s="14"/>
       <c r="C26" s="10" t="s">
         <v>30</v>
@@ -1059,7 +1175,7 @@
       <c r="H26" s="15"/>
       <c r="I26" s="16"/>
     </row>
-    <row r="27" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B27" s="14"/>
       <c r="C27" s="10" t="s">
         <v>31</v>
@@ -1079,7 +1195,7 @@
       <c r="H27" s="15"/>
       <c r="I27" s="16"/>
     </row>
-    <row r="28" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B28" s="14"/>
       <c r="C28" s="10" t="s">
         <v>32</v>
@@ -1099,7 +1215,7 @@
       <c r="H28" s="15"/>
       <c r="I28" s="16"/>
     </row>
-    <row r="29" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B29" s="14"/>
       <c r="C29" s="10" t="s">
         <v>33</v>
@@ -1119,7 +1235,7 @@
       <c r="H29" s="15"/>
       <c r="I29" s="16"/>
     </row>
-    <row r="30" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B30" s="14"/>
       <c r="C30" s="10" t="s">
         <v>34</v>
@@ -1139,7 +1255,7 @@
       <c r="H30" s="15"/>
       <c r="I30" s="16"/>
     </row>
-    <row r="31" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B31" s="14"/>
       <c r="C31" s="13" t="s">
         <v>40</v>
@@ -1153,7 +1269,7 @@
       <c r="H31" s="15"/>
       <c r="I31" s="16"/>
     </row>
-    <row r="32" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B32" s="4"/>
       <c r="C32" s="5"/>
       <c r="D32" s="5"/>
@@ -1163,6 +1279,265 @@
       <c r="H32" s="5"/>
       <c r="I32" s="6"/>
     </row>
+    <row r="34" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="35" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B35" s="1"/>
+      <c r="C35" s="2"/>
+      <c r="D35" s="2"/>
+      <c r="E35" s="2"/>
+      <c r="F35" s="2"/>
+      <c r="G35" s="2"/>
+      <c r="H35" s="2"/>
+      <c r="I35" s="3"/>
+    </row>
+    <row r="36" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B36" s="14"/>
+      <c r="C36" s="10" t="s">
+        <v>54</v>
+      </c>
+      <c r="D36" s="10" t="s">
+        <v>60</v>
+      </c>
+      <c r="E36" s="15"/>
+      <c r="F36" s="15"/>
+      <c r="G36" s="15"/>
+      <c r="H36" s="15"/>
+      <c r="I36" s="16"/>
+    </row>
+    <row r="37" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B37" s="14"/>
+      <c r="C37" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="D37" s="10" t="s">
+        <v>61</v>
+      </c>
+      <c r="E37" s="15"/>
+      <c r="F37" s="15"/>
+      <c r="G37" s="15"/>
+      <c r="H37" s="15"/>
+      <c r="I37" s="16"/>
+    </row>
+    <row r="38" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B38" s="14"/>
+      <c r="C38" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="D38" s="10" t="s">
+        <v>62</v>
+      </c>
+      <c r="E38" s="15"/>
+      <c r="F38" s="15"/>
+      <c r="G38" s="15"/>
+      <c r="H38" s="15"/>
+      <c r="I38" s="16"/>
+    </row>
+    <row r="39" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B39" s="14"/>
+      <c r="C39" s="15"/>
+      <c r="D39" s="15"/>
+      <c r="E39" s="15"/>
+      <c r="F39" s="15"/>
+      <c r="G39" s="15"/>
+      <c r="H39" s="15"/>
+      <c r="I39" s="16"/>
+    </row>
+    <row r="40" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B40" s="14"/>
+      <c r="C40" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="D40" s="15"/>
+      <c r="E40" s="15"/>
+      <c r="F40" s="15"/>
+      <c r="G40" s="15"/>
+      <c r="H40" s="15"/>
+      <c r="I40" s="16"/>
+    </row>
+    <row r="41" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B41" s="14"/>
+      <c r="C41" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="D41" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="E41" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="F41" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="G41" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="H41" s="15"/>
+      <c r="I41" s="16"/>
+    </row>
+    <row r="42" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B42" s="14"/>
+      <c r="C42" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="D42" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="E42" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="F42" s="12"/>
+      <c r="G42" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="H42" s="15"/>
+      <c r="I42" s="16"/>
+    </row>
+    <row r="43" spans="2:9" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B43" s="14"/>
+      <c r="C43" s="10"/>
+      <c r="D43" s="10"/>
+      <c r="E43" s="10"/>
+      <c r="F43" s="10"/>
+      <c r="G43" s="11"/>
+      <c r="H43" s="15"/>
+      <c r="I43" s="16"/>
+    </row>
+    <row r="44" spans="2:9" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B44" s="14"/>
+      <c r="C44" s="10"/>
+      <c r="D44" s="10"/>
+      <c r="E44" s="10"/>
+      <c r="F44" s="10"/>
+      <c r="G44" s="11"/>
+      <c r="H44" s="15"/>
+      <c r="I44" s="16"/>
+    </row>
+    <row r="45" spans="2:9" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B45" s="14"/>
+      <c r="C45" s="10"/>
+      <c r="D45" s="10"/>
+      <c r="E45" s="10"/>
+      <c r="F45" s="10"/>
+      <c r="G45" s="11"/>
+      <c r="H45" s="15"/>
+      <c r="I45" s="16"/>
+    </row>
+    <row r="46" spans="2:9" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B46" s="14"/>
+      <c r="C46" s="10"/>
+      <c r="D46" s="10"/>
+      <c r="E46" s="10"/>
+      <c r="F46" s="10"/>
+      <c r="G46" s="11"/>
+      <c r="H46" s="15"/>
+      <c r="I46" s="16"/>
+    </row>
+    <row r="47" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B47" s="14"/>
+      <c r="C47" s="13" t="s">
+        <v>40</v>
+      </c>
+      <c r="D47" s="10"/>
+      <c r="E47" s="10"/>
+      <c r="F47" s="15"/>
+      <c r="G47" s="15"/>
+      <c r="H47" s="15"/>
+      <c r="I47" s="16"/>
+    </row>
+    <row r="48" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B48" s="4"/>
+      <c r="C48" s="5"/>
+      <c r="D48" s="5"/>
+      <c r="E48" s="5"/>
+      <c r="F48" s="5"/>
+      <c r="G48" s="5"/>
+      <c r="H48" s="5"/>
+      <c r="I48" s="6"/>
+    </row>
+    <row r="53" spans="3:7" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="54" spans="3:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C54" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="D54" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="E54" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="F54" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="G54" s="9" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="55" spans="3:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C55" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="D55" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="E55" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="F55" s="12"/>
+      <c r="G55" s="12" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="56" spans="3:7" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C56" s="18" t="s">
+        <v>66</v>
+      </c>
+      <c r="D56" s="17" t="s">
+        <v>63</v>
+      </c>
+      <c r="E56" s="17" t="s">
+        <v>65</v>
+      </c>
+      <c r="F56" s="10"/>
+      <c r="G56" s="11" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="57" spans="3:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C57" s="22" t="s">
+        <v>70</v>
+      </c>
+      <c r="D57" s="19" t="s">
+        <v>67</v>
+      </c>
+      <c r="E57" s="20" t="s">
+        <v>68</v>
+      </c>
+      <c r="F57" s="10"/>
+      <c r="G57" s="21" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="58" spans="3:7" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C58" s="22" t="s">
+        <v>72</v>
+      </c>
+      <c r="D58" s="17" t="s">
+        <v>71</v>
+      </c>
+      <c r="E58" s="17" t="s">
+        <v>68</v>
+      </c>
+      <c r="F58" s="10"/>
+      <c r="G58" s="21" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="59" spans="3:7" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="C59" s="10"/>
+      <c r="E59" s="10"/>
+      <c r="F59" s="10"/>
+      <c r="G59" s="11"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>

</xml_diff>